<commit_message>
new kernels fisher vector ongoing
</commit_message>
<xml_diff>
--- a/todo-list.xlsx
+++ b/todo-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hippolyte/Desktop/MVA/Kernel methods/Kaggle-KM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hippolyte/Projects/Kaggle-KM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F6181B-5146-C247-9250-744B80145633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD55303-D9C8-8744-AF80-D44DBCDF1ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="0" windowWidth="34600" windowHeight="28800" xr2:uid="{19A0A20A-D9F1-0844-93F0-7B69648C03D3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16380" xr2:uid="{19A0A20A-D9F1-0844-93F0-7B69648C03D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Kernels</t>
   </si>
@@ -115,6 +115,15 @@
 Section 7.4
 Example of algorithm: https://www.jmlr.org/papers/volume7/sonnenburg06a/sonnenburg06a.pdf
 Implementation: https://github.com/xnevs/msvm/blob/master/msvm.py</t>
+  </si>
+  <si>
+    <t>Sigmoid kernel</t>
+  </si>
+  <si>
+    <t>Laplacian kernel</t>
+  </si>
+  <si>
+    <t>PCA</t>
   </si>
 </sst>
 </file>
@@ -138,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -351,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -365,6 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,9 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -715,7 +732,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +742,9 @@
     <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="124.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -744,8 +763,12 @@
       <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -755,10 +778,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="8"/>
@@ -773,7 +796,7 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
@@ -789,8 +812,8 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="9"/>
@@ -805,7 +828,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
@@ -823,7 +846,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
       <c r="D7" s="2"/>
@@ -837,7 +860,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2"/>
@@ -851,7 +874,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="12"/>
       <c r="C9" s="9"/>
       <c r="D9" s="2"/>
@@ -865,7 +888,7 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -883,7 +906,7 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
@@ -896,12 +919,12 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -917,7 +940,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
@@ -935,8 +958,10 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -949,7 +974,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
       <c r="D15" s="2"/>
@@ -963,7 +988,7 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
       <c r="D16" s="2"/>
@@ -977,7 +1002,7 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="12"/>
       <c r="C17" s="9"/>
       <c r="D17" s="2"/>
@@ -991,10 +1016,10 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="9"/>
@@ -1009,8 +1034,8 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="9"/>
@@ -1025,7 +1050,7 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
@@ -1043,7 +1068,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="11" t="s">
         <v>23</v>
       </c>
@@ -1056,12 +1081,12 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
       <c r="D22" s="2"/>
@@ -1075,7 +1100,7 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
       <c r="D23" s="2"/>
@@ -1089,7 +1114,7 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
       <c r="D24" s="2"/>
@@ -1103,7 +1128,7 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
       <c r="D25" s="2"/>
@@ -1117,7 +1142,7 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
       <c r="D26" s="2"/>
@@ -1131,7 +1156,7 @@
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
       <c r="D27" s="2"/>
@@ -1145,7 +1170,7 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
       <c r="D28" s="2"/>
@@ -1159,7 +1184,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
       <c r="D29" s="2"/>

</xml_diff>

<commit_message>
Experiments pipeline + minor bug fixed
</commit_message>
<xml_diff>
--- a/todo-list.xlsx
+++ b/todo-list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hippolyte/Projects/Kaggle-KM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hippolyte/Desktop/Projects/Kaggle-KM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2204A5-D061-884F-A2BA-2DFAE410BF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12D2241-D001-1C46-8DD6-15299EC81DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16280" xr2:uid="{19A0A20A-D9F1-0844-93F0-7B69648C03D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Kernels</t>
   </si>
@@ -136,6 +136,72 @@
   </si>
   <si>
     <t>Find the optimal set of features, then plot the Explained variance as a func of ,number of components to determine the best kernel for PCA and then test best kernel for SVM</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>CVXOPT</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Raw features</t>
+  </si>
+  <si>
+    <t>Bow features</t>
+  </si>
+  <si>
+    <t>FIsherVect features</t>
+  </si>
+  <si>
+    <t>Dim PCA without norm</t>
+  </si>
+  <si>
+    <t>Dim PCA with norm</t>
+  </si>
+  <si>
+    <t>Kernel PCA</t>
+  </si>
+  <si>
+    <t>Kernel SVM</t>
+  </si>
+  <si>
+    <t>Combinaison</t>
+  </si>
+  <si>
+    <t>RBF parameter for PCA</t>
+  </si>
+  <si>
+    <t>RBF parameter for SVM</t>
+  </si>
+  <si>
+    <t>Chi2 parameter for PCA</t>
+  </si>
+  <si>
+    <t>Chi2 parameter for SVM</t>
+  </si>
+  <si>
+    <t>Laplacian parameter for SVM</t>
+  </si>
+  <si>
+    <t>Laplacian parameter for PCA</t>
+  </si>
+  <si>
+    <t>k on Fisher vect</t>
+  </si>
+  <si>
+    <t>k on BoW</t>
+  </si>
+  <si>
+    <t>Impact of C on linear SVM</t>
+  </si>
+  <si>
+    <t>Impact of C on gaussian SCM</t>
   </si>
 </sst>
 </file>
@@ -198,7 +264,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.749992370372631"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,7 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -771,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5360646-32FE-874F-A1B2-1F28AA6F3876}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,11 +854,14 @@
     <col min="7" max="7" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="124.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -818,9 +887,15 @@
       <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="N2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -836,10 +911,14 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="24" t="s">
+      <c r="N3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="23"/>
+      <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="9"/>
@@ -852,9 +931,13 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="N4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="23"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -868,9 +951,13 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="N5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="23"/>
       <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
@@ -886,9 +973,13 @@
       <c r="L6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
+      <c r="N6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="23"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
       <c r="D7" s="2"/>
@@ -900,9 +991,13 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="N7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2"/>
@@ -914,9 +1009,13 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="N8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
       <c r="B9" s="12"/>
       <c r="C9" s="9"/>
       <c r="D9" s="2"/>
@@ -928,9 +1027,13 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="N9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -946,10 +1049,14 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="20" t="s">
+      <c r="N10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="9"/>
@@ -964,10 +1071,14 @@
       <c r="L11" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24" t="s">
+      <c r="N11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="9"/>
@@ -980,9 +1091,13 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="N12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
       <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
@@ -998,9 +1113,13 @@
       <c r="L13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="N13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
       <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
@@ -1014,9 +1133,13 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
+      <c r="N14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
       <c r="D15" s="2"/>
@@ -1028,9 +1151,13 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="N15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="23"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
       <c r="D16" s="2"/>
@@ -1042,9 +1169,13 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="N16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
       <c r="B17" s="12"/>
       <c r="C17" s="9"/>
       <c r="D17" s="2"/>
@@ -1056,9 +1187,13 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="N17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1074,9 +1209,13 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
+      <c r="N18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
       <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
@@ -1090,9 +1229,13 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
+      <c r="N19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="23"/>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
@@ -1108,9 +1251,13 @@
       <c r="L20" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
+      <c r="N20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
       <c r="B21" s="20" t="s">
         <v>23</v>
       </c>
@@ -1126,9 +1273,13 @@
       <c r="L21" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
+      <c r="N21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9"/>
       <c r="D22" s="2"/>
@@ -1140,9 +1291,13 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
+      <c r="N22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9"/>
       <c r="D23" s="2"/>
@@ -1155,8 +1310,8 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="23"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
       <c r="D24" s="2"/>
@@ -1169,8 +1324,8 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="23"/>
       <c r="B25" s="11"/>
       <c r="C25" s="9"/>
       <c r="D25" s="2"/>
@@ -1183,8 +1338,8 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="23"/>
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
       <c r="D26" s="2"/>
@@ -1197,8 +1352,8 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
       <c r="D27" s="2"/>
@@ -1211,8 +1366,8 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="23"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
       <c r="D28" s="2"/>
@@ -1225,8 +1380,8 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+    <row r="29" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
       <c r="D29" s="2"/>
@@ -1239,7 +1394,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>